<commit_message>
update to the dark mode
</commit_message>
<xml_diff>
--- a/Pendientes.xlsx
+++ b/Pendientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USUARIOS\Desktop\OST\PlataformaComercio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1438217-E2EE-4CC6-A9BE-4631F97CA618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3EEA90-ABF9-4923-9684-F7C279A82A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Backend</t>
   </si>
@@ -158,9 +158,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -177,6 +174,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,7 +462,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,44 +470,45 @@
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -515,14 +516,18 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="1"/>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -530,14 +535,14 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>10</v>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -545,14 +550,14 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -563,7 +568,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -574,7 +579,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>